<commit_message>
prior to fastq convert
</commit_message>
<xml_diff>
--- a/RIpanel.Brain/documents/analysisProgress.brain.xlsx
+++ b/RIpanel.Brain/documents/analysisProgress.brain.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="10320" windowHeight="15640" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="13580" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="54">
   <si>
     <t>SHR_1</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>converted to fastq</t>
-  </si>
-  <si>
-    <t>partial</t>
   </si>
   <si>
     <t>running</t>
@@ -215,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,12 +222,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,7 +247,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -294,19 +285,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -325,6 +327,12 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -343,6 +351,12 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -674,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -683,217 +697,217 @@
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="45">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="45">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -901,27 +915,27 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -937,16 +951,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -954,31 +968,31 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>19</v>
+      <c r="B26" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>18</v>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>18</v>
+      <c r="B28" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -986,7 +1000,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -994,7 +1008,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1002,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1010,39 +1024,39 @@
         <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>19</v>
+      <c r="B33" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>19</v>
+      <c r="B34" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>19</v>
+      <c r="B35" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>19</v>
+      <c r="B36" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1050,64 +1064,64 @@
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>19</v>
+      <c r="B38" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>18</v>
@@ -1115,23 +1129,23 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>18</v>
@@ -1139,58 +1153,58 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>33</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>27</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>34</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>28</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>20</v>
+      <c r="B58" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>